<commit_message>
Daily attendance processing - 2026-02-06 11:37:41 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y3_B2526_Urogenital_session_analysis.xlsx
+++ b/attendance_reports/Y3_B2526_Urogenital_session_analysis.xlsx
@@ -81,7 +81,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -100,6 +100,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -481,7 +484,7 @@
     <col width="9" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="13" customWidth="1" min="7" max="7"/>
+    <col width="28" customWidth="1" min="7" max="7"/>
     <col width="10" customWidth="1" min="8" max="8"/>
     <col width="14" customWidth="1" min="9" max="9"/>
     <col width="22" customWidth="1" min="11" max="11"/>
@@ -793,7 +796,7 @@
         </is>
       </c>
       <c r="L6" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -844,7 +847,7 @@
         </is>
       </c>
       <c r="L7" s="4" t="n">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8">
@@ -947,7 +950,7 @@
       </c>
       <c r="L9" s="4" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>0.9%</t>
         </is>
       </c>
     </row>
@@ -1000,7 +1003,7 @@
       </c>
       <c r="L10" s="4" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>8.3%</t>
         </is>
       </c>
     </row>
@@ -1363,22 +1366,22 @@
         <v>19</v>
       </c>
       <c r="O16" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P16" s="4" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q16" s="4" t="n">
         <v>0</v>
       </c>
       <c r="R16" s="4" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>5.3%</t>
         </is>
       </c>
       <c r="S16" s="4" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>8.3%</t>
         </is>
       </c>
     </row>
@@ -2061,45 +2064,49 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="2" t="inlineStr">
-        <is>
-          <t>Year 3</t>
-        </is>
-      </c>
-      <c r="B28" s="2" t="inlineStr">
+      <c r="A28" s="8" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B28" s="8" t="inlineStr">
         <is>
           <t>A2</t>
         </is>
       </c>
-      <c r="C28" s="2" t="inlineStr">
+      <c r="C28" s="8" t="inlineStr">
         <is>
           <t>MICROBIOLOGY</t>
         </is>
       </c>
-      <c r="D28" s="2" t="inlineStr">
+      <c r="D28" s="8" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E28" s="2" t="inlineStr">
+      <c r="E28" s="8" t="inlineStr">
         <is>
           <t>23/11/2025</t>
         </is>
       </c>
-      <c r="F28" s="2" t="inlineStr">
+      <c r="F28" s="8" t="inlineStr">
         <is>
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G28" s="2" t="inlineStr"/>
-      <c r="H28" s="2" t="inlineStr">
-        <is>
-          <t>0/204</t>
-        </is>
-      </c>
-      <c r="I28" s="2" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="G28" s="8" t="inlineStr">
+        <is>
+          <t>sara_atawia@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="H28" s="8" t="inlineStr">
+        <is>
+          <t>17/204</t>
+        </is>
+      </c>
+      <c r="I28" s="8" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-09 08:12:00 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y3_B2526_Urogenital_session_analysis.xlsx
+++ b/attendance_reports/Y3_B2526_Urogenital_session_analysis.xlsx
@@ -1003,7 +1003,7 @@
       </c>
       <c r="L10" s="4" t="inlineStr">
         <is>
-          <t>40.8%</t>
+          <t>40.9%</t>
         </is>
       </c>
     </row>
@@ -1619,7 +1619,7 @@
       </c>
       <c r="S19" s="4" t="inlineStr">
         <is>
-          <t>34.0%</t>
+          <t>34.4%</t>
         </is>
       </c>
     </row>
@@ -2966,7 +2966,11 @@
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G48" s="2" t="inlineStr"/>
+      <c r="G48" s="2" t="inlineStr">
+        <is>
+          <t>maimustafa@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H48" s="2" t="inlineStr">
         <is>
           <t>93/216</t>
@@ -4608,10 +4612,14 @@
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G86" s="2" t="inlineStr"/>
+      <c r="G86" s="2" t="inlineStr">
+        <is>
+          <t>maimustafa@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H86" s="2" t="inlineStr">
         <is>
-          <t>34/227</t>
+          <t>54/227</t>
         </is>
       </c>
       <c r="I86" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-12 05:57:55 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y3_B2526_Urogenital_session_analysis.xlsx
+++ b/attendance_reports/Y3_B2526_Urogenital_session_analysis.xlsx
@@ -93,9 +93,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -103,6 +100,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -796,7 +796,7 @@
         </is>
       </c>
       <c r="L6" s="4" t="n">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7">
@@ -847,49 +847,53 @@
         </is>
       </c>
       <c r="L7" s="4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="inlineStr">
-        <is>
-          <t>Year 3</t>
-        </is>
-      </c>
-      <c r="B8" s="5" t="inlineStr">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
         <is>
           <t>A1</t>
         </is>
       </c>
-      <c r="C8" s="5" t="inlineStr">
+      <c r="C8" s="2" t="inlineStr">
         <is>
           <t>HISTOLOGY</t>
         </is>
       </c>
-      <c r="D8" s="5" t="inlineStr">
+      <c r="D8" s="2" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="E8" s="5" t="inlineStr">
+      <c r="E8" s="2" t="inlineStr">
         <is>
           <t>14/12/2025</t>
         </is>
       </c>
-      <c r="F8" s="5" t="inlineStr">
+      <c r="F8" s="2" t="inlineStr">
         <is>
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G8" s="5" t="inlineStr"/>
-      <c r="H8" s="5" t="inlineStr">
-        <is>
-          <t>0/203</t>
-        </is>
-      </c>
-      <c r="I8" s="5" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="G8" s="2" t="inlineStr">
+        <is>
+          <t>aya.saeed@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="H8" s="2" t="inlineStr">
+        <is>
+          <t>72/203</t>
+        </is>
+      </c>
+      <c r="I8" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
       <c r="K8" s="4" t="inlineStr">
@@ -950,7 +954,7 @@
       </c>
       <c r="L9" s="4" t="inlineStr">
         <is>
-          <t>91.2%</t>
+          <t>92.1%</t>
         </is>
       </c>
     </row>
@@ -1292,22 +1296,22 @@
         <v>19</v>
       </c>
       <c r="O15" s="4" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P15" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q15" s="4" t="n">
         <v>0</v>
       </c>
       <c r="R15" s="4" t="inlineStr">
         <is>
-          <t>94.7%</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="S15" s="4" t="inlineStr">
         <is>
-          <t>40.8%</t>
+          <t>40.5%</t>
         </is>
       </c>
     </row>
@@ -1944,7 +1948,7 @@
           <t>Recorded</t>
         </is>
       </c>
-      <c r="L25" s="6" t="inlineStr">
+      <c r="L25" s="5" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -2002,7 +2006,7 @@
           <t>Not Recorded</t>
         </is>
       </c>
-      <c r="L26" s="7" t="inlineStr">
+      <c r="L26" s="6" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -2060,7 +2064,7 @@
           <t>Pending</t>
         </is>
       </c>
-      <c r="L27" s="8" t="inlineStr">
+      <c r="L27" s="7" t="inlineStr">
         <is>
           <t>Yellow</t>
         </is>
@@ -2381,43 +2385,43 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="5" t="inlineStr">
-        <is>
-          <t>Year 3</t>
-        </is>
-      </c>
-      <c r="B35" s="5" t="inlineStr">
+      <c r="A35" s="8" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B35" s="8" t="inlineStr">
         <is>
           <t>A2</t>
         </is>
       </c>
-      <c r="C35" s="5" t="inlineStr">
+      <c r="C35" s="8" t="inlineStr">
         <is>
           <t>PHARMACOLOGY</t>
         </is>
       </c>
-      <c r="D35" s="5" t="inlineStr">
+      <c r="D35" s="8" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E35" s="5" t="inlineStr">
+      <c r="E35" s="8" t="inlineStr">
         <is>
           <t>30/11/2025</t>
         </is>
       </c>
-      <c r="F35" s="5" t="inlineStr">
+      <c r="F35" s="8" t="inlineStr">
         <is>
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G35" s="5" t="inlineStr"/>
-      <c r="H35" s="5" t="inlineStr">
+      <c r="G35" s="8" t="inlineStr"/>
+      <c r="H35" s="8" t="inlineStr">
         <is>
           <t>0/204</t>
         </is>
       </c>
-      <c r="I35" s="5" t="inlineStr">
+      <c r="I35" s="8" t="inlineStr">
         <is>
           <t>Not Recorded</t>
         </is>
@@ -2888,7 +2892,11 @@
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G46" s="2" t="inlineStr"/>
+      <c r="G46" s="2" t="inlineStr">
+        <is>
+          <t>aya.saeed@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
           <t>21/216</t>
@@ -3257,43 +3265,43 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="5" t="inlineStr">
-        <is>
-          <t>Year 3</t>
-        </is>
-      </c>
-      <c r="B55" s="5" t="inlineStr">
+      <c r="A55" s="8" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B55" s="8" t="inlineStr">
         <is>
           <t>A3</t>
         </is>
       </c>
-      <c r="C55" s="5" t="inlineStr">
+      <c r="C55" s="8" t="inlineStr">
         <is>
           <t>PHARMACOLOGY</t>
         </is>
       </c>
-      <c r="D55" s="5" t="inlineStr">
+      <c r="D55" s="8" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E55" s="5" t="inlineStr">
+      <c r="E55" s="8" t="inlineStr">
         <is>
           <t>11/12/2025</t>
         </is>
       </c>
-      <c r="F55" s="5" t="inlineStr">
+      <c r="F55" s="8" t="inlineStr">
         <is>
           <t>12:00:00</t>
         </is>
       </c>
-      <c r="G55" s="5" t="inlineStr"/>
-      <c r="H55" s="5" t="inlineStr">
+      <c r="G55" s="8" t="inlineStr"/>
+      <c r="H55" s="8" t="inlineStr">
         <is>
           <t>0/216</t>
         </is>
       </c>
-      <c r="I55" s="5" t="inlineStr">
+      <c r="I55" s="8" t="inlineStr">
         <is>
           <t>Not Recorded</t>
         </is>
@@ -3558,43 +3566,43 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="5" t="inlineStr">
-        <is>
-          <t>Year 3</t>
-        </is>
-      </c>
-      <c r="B62" s="5" t="inlineStr">
+      <c r="A62" s="8" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B62" s="8" t="inlineStr">
         <is>
           <t>B1</t>
         </is>
       </c>
-      <c r="C62" s="5" t="inlineStr">
+      <c r="C62" s="8" t="inlineStr">
         <is>
           <t>BIOCHEMISTRY LAB/CBL</t>
         </is>
       </c>
-      <c r="D62" s="5" t="inlineStr">
+      <c r="D62" s="8" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E62" s="5" t="inlineStr">
+      <c r="E62" s="8" t="inlineStr">
         <is>
           <t>13/11/2025</t>
         </is>
       </c>
-      <c r="F62" s="5" t="inlineStr">
+      <c r="F62" s="8" t="inlineStr">
         <is>
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G62" s="5" t="inlineStr"/>
-      <c r="H62" s="5" t="inlineStr">
+      <c r="G62" s="8" t="inlineStr"/>
+      <c r="H62" s="8" t="inlineStr">
         <is>
           <t>0/149</t>
         </is>
       </c>
-      <c r="I62" s="5" t="inlineStr">
+      <c r="I62" s="8" t="inlineStr">
         <is>
           <t>Not Recorded</t>
         </is>
@@ -3902,43 +3910,43 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="5" t="inlineStr">
-        <is>
-          <t>Year 3</t>
-        </is>
-      </c>
-      <c r="B70" s="5" t="inlineStr">
+      <c r="A70" s="8" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B70" s="8" t="inlineStr">
         <is>
           <t>B1</t>
         </is>
       </c>
-      <c r="C70" s="5" t="inlineStr">
+      <c r="C70" s="8" t="inlineStr">
         <is>
           <t>PATHOLOGY LAB/MUSEUM</t>
         </is>
       </c>
-      <c r="D70" s="5" t="inlineStr">
+      <c r="D70" s="8" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E70" s="5" t="inlineStr">
+      <c r="E70" s="8" t="inlineStr">
         <is>
           <t>11/12/2025</t>
         </is>
       </c>
-      <c r="F70" s="5" t="inlineStr">
+      <c r="F70" s="8" t="inlineStr">
         <is>
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G70" s="5" t="inlineStr"/>
-      <c r="H70" s="5" t="inlineStr">
+      <c r="G70" s="8" t="inlineStr"/>
+      <c r="H70" s="8" t="inlineStr">
         <is>
           <t>0/149</t>
         </is>
       </c>
-      <c r="I70" s="5" t="inlineStr">
+      <c r="I70" s="8" t="inlineStr">
         <is>
           <t>Not Recorded</t>
         </is>
@@ -5501,86 +5509,86 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="5" t="inlineStr">
-        <is>
-          <t>Year 3</t>
-        </is>
-      </c>
-      <c r="B107" s="5" t="inlineStr">
+      <c r="A107" s="8" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B107" s="8" t="inlineStr">
         <is>
           <t>B3</t>
         </is>
       </c>
-      <c r="C107" s="5" t="inlineStr">
+      <c r="C107" s="8" t="inlineStr">
         <is>
           <t>PATHOLOGY LAB/MUSEUM</t>
         </is>
       </c>
-      <c r="D107" s="5" t="inlineStr">
+      <c r="D107" s="8" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E107" s="5" t="inlineStr">
+      <c r="E107" s="8" t="inlineStr">
         <is>
           <t>03/12/2025</t>
         </is>
       </c>
-      <c r="F107" s="5" t="inlineStr">
+      <c r="F107" s="8" t="inlineStr">
         <is>
           <t>12:00:00</t>
         </is>
       </c>
-      <c r="G107" s="5" t="inlineStr"/>
-      <c r="H107" s="5" t="inlineStr">
+      <c r="G107" s="8" t="inlineStr"/>
+      <c r="H107" s="8" t="inlineStr">
         <is>
           <t>0/220</t>
         </is>
       </c>
-      <c r="I107" s="5" t="inlineStr">
+      <c r="I107" s="8" t="inlineStr">
         <is>
           <t>Not Recorded</t>
         </is>
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="5" t="inlineStr">
-        <is>
-          <t>Year 3</t>
-        </is>
-      </c>
-      <c r="B108" s="5" t="inlineStr">
+      <c r="A108" s="8" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B108" s="8" t="inlineStr">
         <is>
           <t>B3</t>
         </is>
       </c>
-      <c r="C108" s="5" t="inlineStr">
+      <c r="C108" s="8" t="inlineStr">
         <is>
           <t>PATHOLOGY LAB/MUSEUM</t>
         </is>
       </c>
-      <c r="D108" s="5" t="inlineStr">
+      <c r="D108" s="8" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E108" s="5" t="inlineStr">
+      <c r="E108" s="8" t="inlineStr">
         <is>
           <t>10/12/2025</t>
         </is>
       </c>
-      <c r="F108" s="5" t="inlineStr">
+      <c r="F108" s="8" t="inlineStr">
         <is>
           <t>12:00:00</t>
         </is>
       </c>
-      <c r="G108" s="5" t="inlineStr"/>
-      <c r="H108" s="5" t="inlineStr">
+      <c r="G108" s="8" t="inlineStr"/>
+      <c r="H108" s="8" t="inlineStr">
         <is>
           <t>0/220</t>
         </is>
       </c>
-      <c r="I108" s="5" t="inlineStr">
+      <c r="I108" s="8" t="inlineStr">
         <is>
           <t>Not Recorded</t>
         </is>
@@ -5681,86 +5689,86 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="5" t="inlineStr">
-        <is>
-          <t>Year 3</t>
-        </is>
-      </c>
-      <c r="B111" s="5" t="inlineStr">
+      <c r="A111" s="8" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B111" s="8" t="inlineStr">
         <is>
           <t>B3</t>
         </is>
       </c>
-      <c r="C111" s="5" t="inlineStr">
+      <c r="C111" s="8" t="inlineStr">
         <is>
           <t>PHARMACOLOGY</t>
         </is>
       </c>
-      <c r="D111" s="5" t="inlineStr">
+      <c r="D111" s="8" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E111" s="5" t="inlineStr">
+      <c r="E111" s="8" t="inlineStr">
         <is>
           <t>04/12/2025</t>
         </is>
       </c>
-      <c r="F111" s="5" t="inlineStr">
+      <c r="F111" s="8" t="inlineStr">
         <is>
           <t>12:00:00</t>
         </is>
       </c>
-      <c r="G111" s="5" t="inlineStr"/>
-      <c r="H111" s="5" t="inlineStr">
+      <c r="G111" s="8" t="inlineStr"/>
+      <c r="H111" s="8" t="inlineStr">
         <is>
           <t>0/220</t>
         </is>
       </c>
-      <c r="I111" s="5" t="inlineStr">
+      <c r="I111" s="8" t="inlineStr">
         <is>
           <t>Not Recorded</t>
         </is>
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="5" t="inlineStr">
-        <is>
-          <t>Year 3</t>
-        </is>
-      </c>
-      <c r="B112" s="5" t="inlineStr">
+      <c r="A112" s="8" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B112" s="8" t="inlineStr">
         <is>
           <t>B3</t>
         </is>
       </c>
-      <c r="C112" s="5" t="inlineStr">
+      <c r="C112" s="8" t="inlineStr">
         <is>
           <t>PHARMACOLOGY</t>
         </is>
       </c>
-      <c r="D112" s="5" t="inlineStr">
+      <c r="D112" s="8" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E112" s="5" t="inlineStr">
+      <c r="E112" s="8" t="inlineStr">
         <is>
           <t>10/12/2025</t>
         </is>
       </c>
-      <c r="F112" s="5" t="inlineStr">
+      <c r="F112" s="8" t="inlineStr">
         <is>
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G112" s="5" t="inlineStr"/>
-      <c r="H112" s="5" t="inlineStr">
+      <c r="G112" s="8" t="inlineStr"/>
+      <c r="H112" s="8" t="inlineStr">
         <is>
           <t>0/220</t>
         </is>
       </c>
-      <c r="I112" s="5" t="inlineStr">
+      <c r="I112" s="8" t="inlineStr">
         <is>
           <t>Not Recorded</t>
         </is>
@@ -5810,43 +5818,43 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="5" t="inlineStr">
-        <is>
-          <t>Year 3</t>
-        </is>
-      </c>
-      <c r="B114" s="5" t="inlineStr">
+      <c r="A114" s="8" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B114" s="8" t="inlineStr">
         <is>
           <t>B3</t>
         </is>
       </c>
-      <c r="C114" s="5" t="inlineStr">
+      <c r="C114" s="8" t="inlineStr">
         <is>
           <t>PHYSIOLOGY</t>
         </is>
       </c>
-      <c r="D114" s="5" t="inlineStr">
+      <c r="D114" s="8" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E114" s="5" t="inlineStr">
+      <c r="E114" s="8" t="inlineStr">
         <is>
           <t>19/11/2025</t>
         </is>
       </c>
-      <c r="F114" s="5" t="inlineStr">
+      <c r="F114" s="8" t="inlineStr">
         <is>
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G114" s="5" t="inlineStr"/>
-      <c r="H114" s="5" t="inlineStr">
+      <c r="G114" s="8" t="inlineStr"/>
+      <c r="H114" s="8" t="inlineStr">
         <is>
           <t>0/220</t>
         </is>
       </c>
-      <c r="I114" s="5" t="inlineStr">
+      <c r="I114" s="8" t="inlineStr">
         <is>
           <t>Not Recorded</t>
         </is>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-12 08:52:51 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y3_B2526_Urogenital_session_analysis.xlsx
+++ b/attendance_reports/Y3_B2526_Urogenital_session_analysis.xlsx
@@ -888,7 +888,7 @@
       </c>
       <c r="H8" s="2" t="inlineStr">
         <is>
-          <t>72/203</t>
+          <t>73/203</t>
         </is>
       </c>
       <c r="I8" s="2" t="inlineStr">
@@ -2899,7 +2899,7 @@
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>21/216</t>
+          <t>22/216</t>
         </is>
       </c>
       <c r="I46" s="2" t="inlineStr">

</xml_diff>